<commit_message>
fix: a fix to point the help URL to the correct document for bulk uploading schemes
AB#181
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Schemes_Template.xlsx
+++ b/public/assets/files/Bulk_Upload_Schemes_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billbatten/Projects/Subsidy/transparency-db-admin-portal/public/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C237B516-3C84-2540-B20D-6F1EA36F56BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4080E01C-31D4-E44D-9C7A-D91B5B293D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{21A0E9DA-93E5-6D4C-A318-074AA844045A}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{21A0E9DA-93E5-6D4C-A318-074AA844045A}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>Public authority name</t>
   </si>
@@ -96,9 +96,6 @@
     <t>This is the name that members of the public will be able to see on 'Search for UK subsidies'</t>
   </si>
   <si>
-    <t>This is a description of the subisy scheme</t>
-  </si>
-  <si>
     <t>This can be a short summary of the policy or economic background of the scheme.</t>
   </si>
   <si>
@@ -108,13 +105,7 @@
     <t>provide a short summary of the page that you have entered the URL for. This will make it easier for other users to understand the contents of the page, without clicking on it.</t>
   </si>
   <si>
-    <t xml:space="preserve">This the budget of the scheme. No awards linked to this scheme will be able to set a budget larger than this. </t>
-  </si>
-  <si>
     <t>This is the date the subsidy scheme was confirmed.</t>
-  </si>
-  <si>
-    <t>This is the date in which the subsidy scheme will start</t>
   </si>
   <si>
     <t xml:space="preserve">This is the maximum amount of money that can be given under any scheme. This is a free text field where the user can add whatever text they want. </t>
@@ -156,13 +147,31 @@
     <t>Limit 5000 characters</t>
   </si>
   <si>
-    <t>1 or more sectors entries should be seperted by a vertical bar "|". E.g   Agriculture, forestry and fishing | Mining and quarrying | Construction</t>
-  </si>
-  <si>
     <t>Limit 255 characters</t>
   </si>
   <si>
-    <t>dd-mmm-yyyy</t>
+    <t>Confirmation date</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>dd-mm-yyyy</t>
+  </si>
+  <si>
+    <t>This is a description of the subsidy scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the budget of the scheme. No awards linked to this scheme will be able to set a budget larger than this. </t>
+  </si>
+  <si>
+    <t>This is the date in which the subsidy scheme will start.</t>
+  </si>
+  <si>
+    <t>1 or more sectors entries should be separted by a vertical bar "|". E.g.   Agriculture, forestry and fishing | Mining and quarrying | Construction</t>
   </si>
 </sst>
 </file>
@@ -622,8 +631,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,13 +677,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -14711,10 +14720,10 @@
         <v>16</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14728,7 +14737,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14739,10 +14748,10 @@
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14753,10 +14762,10 @@
         <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.2">
@@ -14767,10 +14776,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14781,10 +14790,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14795,10 +14804,10 @@
         <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14809,10 +14818,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14823,10 +14832,10 @@
         <v>16</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14837,10 +14846,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -14851,10 +14860,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="408" customHeight="1" x14ac:dyDescent="0.2">
@@ -14865,10 +14874,10 @@
         <v>16</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fixed the bug causing the site to crash when no file was uploads for bulk upload schemes
AB#181
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Schemes_Template.xlsx
+++ b/public/assets/files/Bulk_Upload_Schemes_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billbatten/Projects/Subsidy/transparency-db-admin-portal/public/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4080E01C-31D4-E44D-9C7A-D91B5B293D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B17545C-9481-4443-9B40-3738E3011C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{21A0E9DA-93E5-6D4C-A318-074AA844045A}"/>
   </bookViews>
@@ -111,30 +111,6 @@
     <t xml:space="preserve">This is the maximum amount of money that can be given under any scheme. This is a free text field where the user can add whatever text they want. </t>
   </si>
   <si>
-    <t>Select the Sector where the Award is spent:
-1.Agriculture, forestry and fishing
-2.Mining and quarrying 
-3.Manufacturing 
-4.Electricity, gas, steam and air conditioning supply
-5.Transportation and storage
-6.Wholesale and retail trade; repair of motor vehicles and motorcycles
-7.Construction
-8.Water supply; sewerage, waste management and remediation activities
-9.Accommodation and food service activities
-10.Information and communication
-11.Financial and insurance activities
-12.Real estate activities
-13.Professional, scientific and technical activities
-14.Administrative and support service activities
-15.Public administration and defence; compulsory social security
-16.Education 
-17.Human health and social work activities
-18.Arts, entertainment and recreation
-19.Other service activities
-20.Activities of households as employers; undifferentiated goods- and services-producing activities of households for own use 
-21.Activities of extraterritorial organisations and bodies</t>
-  </si>
-  <si>
     <t>Integer</t>
   </si>
   <si>
@@ -172,6 +148,30 @@
   </si>
   <si>
     <t>1 or more sectors entries should be separted by a vertical bar "|". E.g.   Agriculture, forestry and fishing | Mining and quarrying | Construction</t>
+  </si>
+  <si>
+    <t>Select the Sector where the scheme is spent:
+1.Agriculture, forestry and fishing
+2.Mining and quarrying 
+3.Manufacturing 
+4.Electricity, gas, steam and air conditioning supply
+5.Transportation and storage
+6.Wholesale and retail trade; repair of motor vehicles and motorcycles
+7.Construction
+8.Water supply; sewerage, waste management and remediation activities
+9.Accommodation and food service activities
+10.Information and communication
+11.Financial and insurance activities
+12.Real estate activities
+13.Professional, scientific and technical activities
+14.Administrative and support service activities
+15.Public administration and defence; compulsory social security
+16.Education 
+17.Human health and social work activities
+18.Arts, entertainment and recreation
+19.Other service activities
+20.Activities of households as employers; undifferentiated goods- and services-producing activities of households for own use 
+21.Activities of extraterritorial organisations and bodies</t>
   </si>
 </sst>
 </file>
@@ -677,13 +677,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -14688,7 +14688,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14720,10 +14722,10 @@
         <v>16</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14737,7 +14739,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14748,10 +14750,10 @@
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14765,7 +14767,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.2">
@@ -14779,7 +14781,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14793,7 +14795,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14804,10 +14806,10 @@
         <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14821,7 +14823,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14835,7 +14837,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -14846,10 +14848,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -14860,10 +14862,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="408" customHeight="1" x14ac:dyDescent="0.2">
@@ -14874,10 +14876,10 @@
         <v>16</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added other free text field
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Schemes_Template.xlsx
+++ b/public/assets/files/Bulk_Upload_Schemes_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.robinson\Documents\BEIS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7E7499-A605-4760-9469-3375468F7F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4968FB62-A588-4D92-A100-F642B248B09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{21A0E9DA-93E5-6D4C-A318-074AA844045A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>Public authority name</t>
   </si>
@@ -202,6 +202,12 @@
     <t>Purpose</t>
   </si>
   <si>
+    <t>1 or more purpose(s) should be separted by a vertical bar "|". E.g.  Infrastructure | Regional development | Energy efficiency</t>
+  </si>
+  <si>
+    <t>Purpose - Other</t>
+  </si>
+  <si>
     <t>Select the Purpose of the scheme 
 1.Culture or Heritage
 2.Employment
@@ -211,11 +217,13 @@
 6.Regional development
 7.Rescue and restructuring subsidy
 8.Research and development
-9.Training
-10.Other</t>
+9.Training</t>
   </si>
   <si>
-    <t>1 or more purpose(s) should be separted by a vertical bar "|". E.g.  Infrastructure | Regional development | Energy efficiency</t>
+    <t xml:space="preserve">Enter the Other purpose(s) that are not listed in the purpose field </t>
+  </si>
+  <si>
+    <t>Enter the name of the other purpose. mutliple "Other" entry should be seperated by a comma eg "purpose, another purpose, special purpose"</t>
   </si>
 </sst>
 </file>
@@ -676,9 +684,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912F1757-BE05-7747-AC2A-E7E2F996881E}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N1001"/>
+  <dimension ref="A1:O1001"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -695,10 +705,10 @@
     <col min="11" max="11" width="20.296875" customWidth="1"/>
     <col min="12" max="12" width="22.296875" customWidth="1"/>
     <col min="13" max="13" width="53" customWidth="1"/>
-    <col min="14" max="14" width="37.796875" customWidth="1"/>
+    <col min="14" max="15" width="37.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -741,8 +751,11 @@
       <c r="N1" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -757,7 +770,7 @@
       <c r="L2" s="11"/>
       <c r="M2" s="10"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -772,7 +785,7 @@
       <c r="L3" s="11"/>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -787,7 +800,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -802,7 +815,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -817,7 +830,7 @@
       <c r="L6" s="11"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -832,7 +845,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -847,7 +860,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -862,7 +875,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -877,7 +890,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -892,7 +905,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -907,7 +920,7 @@
       <c r="L12" s="11"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -922,7 +935,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -937,7 +950,7 @@
       <c r="L14" s="11"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -952,7 +965,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -15753,7 +15766,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45C068C-4C31-A44F-A863-7EDDB22D14B7}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
@@ -15961,7 +15974,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="198" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="180" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -15969,10 +15982,24 @@
         <v>16</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="5" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="63" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added legal basis to all awards
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Schemes_Template.xlsx
+++ b/public/assets/files/Bulk_Upload_Schemes_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hajra.hassan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499D2CC1-5E22-443B-8FBC-9B46E4409F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B0F465-FBFA-414B-B967-223300EE58C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{21A0E9DA-93E5-6D4C-A318-074AA844045A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{21A0E9DA-93E5-6D4C-A318-074AA844045A}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -722,9 +722,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>